<commit_message>
Add Python timing results for double Poisson
</commit_message>
<xml_diff>
--- a/CommandLine/Dmitri/ComparingBenchmarks.xlsx
+++ b/CommandLine/Dmitri/ComparingBenchmarks.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmitr\Desktop\xSSIT\CommandLine\Dmitri\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B402A8A-A54D-4CC9-BA5C-3B0A96DD5509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98EFA14-2559-471C-953F-3C42807F4E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ABDA09B7-88D4-4E8D-B98B-46CB9D003C01}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" firstSheet="1" activeTab="2" xr2:uid="{ABDA09B7-88D4-4E8D-B98B-46CB9D003C01}"/>
   </bookViews>
   <sheets>
-    <sheet name="Times" sheetId="1" r:id="rId1"/>
-    <sheet name="Differences " sheetId="2" r:id="rId2"/>
+    <sheet name="Random - Times" sheetId="1" r:id="rId1"/>
+    <sheet name="Random - Differences " sheetId="2" r:id="rId2"/>
+    <sheet name="Poisson - Times" sheetId="3" r:id="rId3"/>
+    <sheet name="Poisson - Differences" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="9">
   <si>
     <t>Expm</t>
   </si>
@@ -237,7 +239,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Times!$A$3:$A$8</c:f>
+              <c:f>'Random - Times'!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -264,7 +266,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Times!$B$3:$B$8</c:f>
+              <c:f>'Random - Times'!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -316,7 +318,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>Times!$A$3:$A$8</c:f>
+              <c:f>'Random - Times'!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -343,7 +345,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Times!$C$3:$C$8</c:f>
+              <c:f>'Random - Times'!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -395,7 +397,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Times!$F$3:$F$8</c:f>
+              <c:f>'Random - Times'!$F$3:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
@@ -447,7 +449,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Times!$G$3:$G$8</c:f>
+              <c:f>'Random - Times'!$G$3:$G$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -516,7 +518,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Times!$A$3:$A$8</c15:sqref>
+                          <c15:sqref>'Random - Times'!$A$3:$A$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -549,7 +551,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>Times!$A$3:$A$8</c15:sqref>
+                          <c15:sqref>'Random - Times'!$A$3:$A$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -965,7 +967,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Differences '!$A$3:$A$8</c:f>
+              <c:f>'Random - Differences '!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -992,7 +994,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Differences '!$B$3:$B$8</c:f>
+              <c:f>'Random - Differences '!$B$3:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1044,7 +1046,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>'Differences '!$A$3:$A$8</c:f>
+              <c:f>'Random - Differences '!$A$3:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1071,7 +1073,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Differences '!$C$3:$C$8</c:f>
+              <c:f>'Random - Differences '!$C$3:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="6"/>
@@ -1122,7 +1124,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Differences '!$A$3:$A$8</c15:sqref>
+                          <c15:sqref>'Random - Differences '!$A$3:$A$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1155,7 +1157,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>'Differences '!$A$3:$A$8</c15:sqref>
+                          <c15:sqref>'Random - Differences '!$A$3:$A$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1187,6 +1189,1255 @@
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-EAEB-4E2D-B599-2D9621D97870}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1124802880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1124802400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1124802400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1124802880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Runtime</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Performance</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>MATLAB expm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Poisson - Times'!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Poisson - Times'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>7.3513399999999996E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.4011599999999995E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.2456400000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.12371198</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27586016000000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1957024999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-0DB7-4278-AC25-EDC24F774CCE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Python expm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Poisson - Times'!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>100</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Poisson - Times'!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>8.0784000001585792E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.21890000000348E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.8072600000086802E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4164400000008699E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1872200000143396E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20323919999964299</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-0DB7-4278-AC25-EDC24F774CCE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>MATLAB ode23s</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Poisson - Times'!$F$3:$F$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.26954E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.03858E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9.2259200000000003E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.1879579999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.7154020000000004E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23747292</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0DB7-4278-AC25-EDC24F774CCE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Python RK23</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Poisson - Times'!$G$3:$G$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>6.2864900000022303E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.3230599999769696E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.9554100000004795E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.5818400000334805E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.9916099999973002E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.20956640000031199</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0DB7-4278-AC25-EDC24F774CCE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1124802880"/>
+        <c:axId val="1124802400"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Number of States</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Poisson - Times'!$A$3:$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00E+00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>100</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Poisson - Times'!$A$3:$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00E+00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>10</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>15</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>25</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>39</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>63</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>100</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-0DB7-4278-AC25-EDC24F774CCE}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1124802880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Number of States</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1124802400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1124802400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Execution</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> time (sec)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1124802880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Georgia" panose="02040502050405020303" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>MATLAB expm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Poisson - Differences'!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Poisson - Differences'!$B$3:$B$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1.6440046542263001E-11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.7733447718805297E-11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.6743107315013799E-11</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.5535907821058999E-11</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.7129881694603498E-11</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.6275113080453406E-11</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-08C3-4CF6-A118-909EFCF83401}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Python expm</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Poisson - Differences'!$A$3:$A$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>251</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>398</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>630</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Poisson - Differences'!$C$3:$C$8</c:f>
+              <c:numCache>
+                <c:formatCode>0.00E+00</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-08C3-4CF6-A118-909EFCF83401}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1124802880"/>
+        <c:axId val="1124802400"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="0"/>
+                <c:order val="0"/>
+                <c:tx>
+                  <c:v>Number of States</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent1"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Poisson - Differences'!$A$3:$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00E+00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>158</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>251</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>398</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>630</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Poisson - Differences'!$A$3:$A$8</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>0.00E+00</c:formatCode>
+                      <c:ptCount val="6"/>
+                      <c:pt idx="0">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>158</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>251</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>398</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>630</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>1000</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-08C3-4CF6-A118-909EFCF83401}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1466,6 +2717,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -1983,6 +3314,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2560,6 +4923,92 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05A2A92E-802D-41EC-B6BB-CD77D857C2A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>100012</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>257175</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DDF740A-AE77-4AC5-85A1-D5369B2CA422}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>157162</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC5681C1-C9A7-4E4F-93C5-AC211024EC5C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2881,8 +5330,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{863BB4CB-418A-42DD-A363-FA4AE93AF3A5}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -3240,4 +5689,387 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A3015D2-B5F8-4D89-A4F3-5035EABD8773}">
+  <dimension ref="A1:G8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>10</v>
+      </c>
+      <c r="B3" s="1">
+        <v>7.3513399999999996E-3</v>
+      </c>
+      <c r="C3" s="3">
+        <v>8.0784000001585792E-3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>4.0506E-4</v>
+      </c>
+      <c r="E3" s="3">
+        <v>8.3528999998634303E-3</v>
+      </c>
+      <c r="F3" s="1">
+        <v>2.26954E-3</v>
+      </c>
+      <c r="G3" s="3">
+        <v>6.2864900000022303E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1">
+        <v>8.4011599999999995E-3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>1.21890000000348E-2</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5.5705999999999996E-4</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1.1345500000061201E-2</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5.03858E-3</v>
+      </c>
+      <c r="G4" s="3">
+        <v>6.3230599999769696E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.2456400000000001E-2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2.8072600000086802E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1.3602E-3</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1.0728499999913699E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <v>9.2259200000000003E-3</v>
+      </c>
+      <c r="G5" s="3">
+        <v>6.9554100000004795E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.12371198</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3.4164400000008699E-2</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1.9926599999999998E-3</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2.6786599999923E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3.1879579999999998E-2</v>
+      </c>
+      <c r="G6" s="3">
+        <v>8.5818400000334805E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>63</v>
+      </c>
+      <c r="B7" s="1">
+        <v>0.27586016000000002</v>
+      </c>
+      <c r="C7" s="3">
+        <v>7.1872200000143396E-2</v>
+      </c>
+      <c r="D7" s="1">
+        <v>3.6414799999999999E-3</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.152870500000062</v>
+      </c>
+      <c r="F7" s="1">
+        <v>7.7154020000000004E-2</v>
+      </c>
+      <c r="G7" s="3">
+        <v>9.9916099999973002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>100</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.1957024999999999</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.20323919999964299</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1.7960340000000002E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.71655969999983404</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.23747292</v>
+      </c>
+      <c r="G8" s="3">
+        <v>0.20956640000031199</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7BE8967-325C-4D6E-A87A-8C83A706F6A0}">
+  <dimension ref="A1:G12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="4"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>100</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1.6440046542263001E-11</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3">
+        <v>4.07778596499764E-5</v>
+      </c>
+      <c r="F3" s="3">
+        <v>4.0777859721149698E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
+        <v>158</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3.7733447718805297E-11</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
+        <v>4.4075411885877199E-5</v>
+      </c>
+      <c r="F4" s="3">
+        <v>4.40754126054382E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
+        <v>251</v>
+      </c>
+      <c r="B5" s="3">
+        <v>4.6743107315013799E-11</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <v>5.66417666304499E-5</v>
+      </c>
+      <c r="F5" s="3">
+        <v>5.6641766398420301E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="3">
+        <v>398</v>
+      </c>
+      <c r="B6" s="3">
+        <v>7.5535907821058999E-11</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <v>7.8285208266258894E-5</v>
+      </c>
+      <c r="F6" s="3">
+        <v>7.8285207031553305E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="3">
+        <v>630</v>
+      </c>
+      <c r="B7" s="3">
+        <v>6.7129881694603498E-11</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <v>8.6707819425442005E-5</v>
+      </c>
+      <c r="F7" s="3">
+        <v>8.6707819707064699E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="3">
+        <v>1000</v>
+      </c>
+      <c r="B8" s="3">
+        <v>7.6275113080453406E-11</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3">
+        <v>8.2559640963690496E-5</v>
+      </c>
+      <c r="F8" s="3">
+        <v>8.2559641070339195E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="3">
+        <v>4.0777859721149698E-5</v>
+      </c>
+      <c r="C12" s="3">
+        <v>4.40754126054382E-5</v>
+      </c>
+      <c r="D12" s="3">
+        <v>5.6641766398420301E-5</v>
+      </c>
+      <c r="E12" s="3">
+        <v>7.8285207031553305E-5</v>
+      </c>
+      <c r="F12" s="3">
+        <v>8.6707819707064699E-5</v>
+      </c>
+      <c r="G12" s="3">
+        <v>8.2559641070339195E-5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>